<commit_message>
added final data for combined barrier
</commit_message>
<xml_diff>
--- a/p2/results/combined_scope.xlsx
+++ b/p2/results/combined_scope.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abauskar/Workspaces/cs6210/p2/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362EF10F-A494-CB44-ADC7-86DFEEB024CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED3E066-D78A-9749-BB72-646C4B8CFA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16280" xr2:uid="{D1336464-EB3B-484F-A1CC-DCAAA50B0548}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D1336464-EB3B-484F-A1CC-DCAAA50B0548}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Processes</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -76,55 +86,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -445,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EE3E182-06FA-434D-8155-3B22B846EC7B}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="K18" sqref="K18:L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -640,15 +611,26 @@
       <c r="F9" s="1">
         <v>10</v>
       </c>
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="B10" s="2">
+        <v>300</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1050</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1160</v>
+      </c>
+      <c r="E10" s="2">
+        <v>442</v>
+      </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -695,15 +677,432 @@
       <c r="A15" s="1">
         <v>12</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <v>2715</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>2</v>
+      </c>
+      <c r="B19" s="1">
+        <v>12</v>
+      </c>
+      <c r="C19" s="1">
+        <v>24</v>
+      </c>
+      <c r="D19">
+        <v>2715</v>
+      </c>
+      <c r="E19">
+        <v>3110</v>
+      </c>
+      <c r="F19">
+        <v>2690</v>
+      </c>
+      <c r="G19">
+        <v>3220</v>
+      </c>
+      <c r="H19">
+        <v>4440</v>
+      </c>
+      <c r="I19">
+        <f>MIN(D19:H19)</f>
+        <v>2690</v>
+      </c>
+      <c r="J19">
+        <f>AVERAGE(D19:H19)</f>
+        <v>3235</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1">
+        <v>10</v>
+      </c>
+      <c r="C20" s="1">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <f>(3200+2940)/2</f>
+        <v>3070</v>
+      </c>
+      <c r="E20">
+        <v>2740</v>
+      </c>
+      <c r="F20">
+        <v>2920</v>
+      </c>
+      <c r="G20">
+        <v>2395</v>
+      </c>
+      <c r="H20">
+        <f>(3090+3290)/2</f>
+        <v>3190</v>
+      </c>
+      <c r="I20">
+        <f t="shared" ref="I20:I30" si="2">MIN(D20:H20)</f>
+        <v>2395</v>
+      </c>
+      <c r="J20">
+        <f t="shared" ref="J20:J30" si="3">AVERAGE(D20:H20)</f>
+        <v>2863</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1">
+        <v>16</v>
+      </c>
+      <c r="D21">
+        <v>1350</v>
+      </c>
+      <c r="E21">
+        <v>1580</v>
+      </c>
+      <c r="F21">
+        <v>2920</v>
+      </c>
+      <c r="G21">
+        <v>1975</v>
+      </c>
+      <c r="H21">
+        <v>1645</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>1350</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="3"/>
+        <v>1894</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1">
+        <v>6</v>
+      </c>
+      <c r="C22" s="1">
+        <v>12</v>
+      </c>
+      <c r="D22">
+        <v>500</v>
+      </c>
+      <c r="E22">
+        <v>485</v>
+      </c>
+      <c r="F22">
+        <v>455</v>
+      </c>
+      <c r="G22">
+        <v>480</v>
+      </c>
+      <c r="H22">
+        <v>510</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>455</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="3"/>
+        <v>486</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1">
+        <v>24</v>
+      </c>
+      <c r="D23">
+        <v>1470</v>
+      </c>
+      <c r="E23">
+        <v>1525</v>
+      </c>
+      <c r="F23">
+        <v>1230</v>
+      </c>
+      <c r="G23">
+        <v>1395</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>1230</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="3"/>
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1">
+        <v>8</v>
+      </c>
+      <c r="D24" s="3">
+        <v>330</v>
+      </c>
+      <c r="E24" s="3">
+        <v>370</v>
+      </c>
+      <c r="F24" s="3">
+        <v>255</v>
+      </c>
+      <c r="G24" s="3">
+        <v>355</v>
+      </c>
+      <c r="H24" s="3">
+        <v>360</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="3"/>
+        <v>334</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1">
+        <v>16</v>
+      </c>
+      <c r="D25" s="3">
+        <v>407</v>
+      </c>
+      <c r="E25" s="3">
+        <v>450</v>
+      </c>
+      <c r="F25" s="3">
+        <v>500</v>
+      </c>
+      <c r="G25" s="3">
+        <v>560</v>
+      </c>
+      <c r="H25" s="3">
+        <v>510</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>407</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="3"/>
+        <v>485.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>5</v>
+      </c>
+      <c r="B26" s="1">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1">
+        <v>9</v>
+      </c>
+      <c r="D26" s="3">
+        <v>750</v>
+      </c>
+      <c r="E26" s="3">
+        <v>790</v>
+      </c>
+      <c r="F26" s="3">
+        <v>680</v>
+      </c>
+      <c r="G26" s="3">
+        <v>860</v>
+      </c>
+      <c r="H26" s="3">
+        <v>940</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>680</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="3"/>
+        <v>804</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>2</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1">
+        <v>4</v>
+      </c>
+      <c r="D27" s="3">
+        <v>350</v>
+      </c>
+      <c r="E27" s="3">
+        <v>360</v>
+      </c>
+      <c r="F27" s="3">
+        <v>250</v>
+      </c>
+      <c r="G27" s="3">
+        <v>240</v>
+      </c>
+      <c r="H27" s="3">
+        <v>225</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="2"/>
+        <v>225</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="3"/>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>4</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2</v>
+      </c>
+      <c r="C28" s="1">
+        <v>8</v>
+      </c>
+      <c r="D28" s="3">
+        <v>390</v>
+      </c>
+      <c r="E28" s="3">
+        <v>310</v>
+      </c>
+      <c r="F28" s="3">
+        <v>840</v>
+      </c>
+      <c r="G28" s="3">
+        <v>280</v>
+      </c>
+      <c r="H28" s="3">
+        <v>300</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="2"/>
+        <v>280</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="3"/>
+        <v>424</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>6</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1">
+        <v>12</v>
+      </c>
+      <c r="D29" s="3">
+        <v>490</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1020</v>
+      </c>
+      <c r="F29" s="3">
+        <v>380</v>
+      </c>
+      <c r="G29" s="3">
+        <v>390</v>
+      </c>
+      <c r="H29" s="3">
+        <v>480</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="2"/>
+        <v>380</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="3"/>
+        <v>552</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>8</v>
+      </c>
+      <c r="B30" s="1">
+        <v>2</v>
+      </c>
+      <c r="C30" s="1">
+        <v>16</v>
+      </c>
+      <c r="D30" s="3">
+        <v>430</v>
+      </c>
+      <c r="E30" s="3">
+        <v>460</v>
+      </c>
+      <c r="F30" s="3">
+        <v>610</v>
+      </c>
+      <c r="G30" s="3">
+        <v>450</v>
+      </c>
+      <c r="H30" s="3">
+        <v>490</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="2"/>
+        <v>430</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="3"/>
+        <v>488</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:F7">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
       <formula>28</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fixup on combined mean
</commit_message>
<xml_diff>
--- a/p2/results/combined_scope.xlsx
+++ b/p2/results/combined_scope.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abauskar/Workspaces/cs6210/p2/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED3E066-D78A-9749-BB72-646C4B8CFA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F49E51-B141-C441-83B6-6A699519F1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D1336464-EB3B-484F-A1CC-DCAAA50B0548}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{D1336464-EB3B-484F-A1CC-DCAAA50B0548}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,7 +419,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18:L18"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,16 +620,16 @@
         <v>2</v>
       </c>
       <c r="B10" s="2">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="C10" s="2">
-        <v>1050</v>
+        <v>424</v>
       </c>
       <c r="D10" s="2">
-        <v>1160</v>
+        <v>552</v>
       </c>
       <c r="E10" s="2">
-        <v>442</v>
+        <v>488</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -637,9 +637,15 @@
       <c r="A11" s="1">
         <v>4</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="B11" s="2">
+        <v>334</v>
+      </c>
+      <c r="C11" s="2">
+        <v>485</v>
+      </c>
+      <c r="D11" s="2">
+        <v>804</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
@@ -647,8 +653,12 @@
       <c r="A12" s="1">
         <v>6</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="2">
+        <v>486</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1405</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -657,7 +667,9 @@
       <c r="A13" s="1">
         <v>8</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <v>1894</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -667,7 +679,9 @@
       <c r="A14" s="1">
         <v>10</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2">
+        <v>2863</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -678,7 +692,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="2">
-        <v>2715</v>
+        <v>3235</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -932,7 +946,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B26" s="1">
         <v>4</v>

</xml_diff>